<commit_message>
Update contract_file from dashboard
</commit_message>
<xml_diff>
--- a/data/data_kontrak_new.xlsx
+++ b/data/data_kontrak_new.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD5610C-B1D0-CD40-BD26-57C6F952BD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71313ED2-635D-1048-9272-0A2EDCCA7A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="1820" windowWidth="27240" windowHeight="16440" xr2:uid="{8AB47025-A3BF-0940-B260-25D870F910D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -674,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF85CBC-8EAD-2144-9BDB-7951ABAA9BFA}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1149,7 +1149,7 @@
         <v>10935</v>
       </c>
       <c r="N10">
-        <v>2187</v>
+        <v>10935</v>
       </c>
       <c r="P10">
         <v>8748</v>

</xml_diff>